<commit_message>
dataset and new models
updated dataset and testing new models
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cemca\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cemca\Desktop\MLR_CarStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87C2358-9BB3-4CC3-9B6B-50EDA362FB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A382CD03-A35F-419E-B5AB-49E756F4E0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3825" yWindow="2160" windowWidth="24915" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,12 +94,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -111,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,12 +127,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,2212 +465,3960 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>0.52950863000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>0.63061118999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>706.71</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>0.52171244999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>703.59</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>658.67</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>2545.33</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>78.86</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>60.94</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>0.52851075999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>700.49</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>656.7</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>2566.46</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>80.23</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>61.25</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>0.52464354999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>699.07</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>662.36</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>2563.52</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>80.930000000000007</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>60.37</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>0.51519594000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>693.82</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>660.14</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>2608.7199999999998</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>84.25</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>60.71</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>0.49589345000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>727.69</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>652.62</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>2463.73</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>71.56</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>61.91</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>0.56165381999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>702.59</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>742</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>2402.44</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>79.28</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>50.89</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>0.65016945999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>712.69</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>725.33</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>2382.9299999999998</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>75.61</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>52.54</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>0.60638174</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>697.32</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>658.03</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>2584.08</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>81.88</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>61.04</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>0.51403147999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>694.99</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>727.86</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>2475.52</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>83.36</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>52.28</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>0.57236547000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>708.72</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>742.85</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>2371.4</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>76.92</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>50.81</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>0.66376679000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>702</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>677.58</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>2516.4899999999998</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>79.540000000000006</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>58.18</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>0.51864522999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>705.21</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>707.21</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>2446.4299999999998</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>78.209999999999994</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>54.5</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>0.55984856000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>696.21</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>646.69000000000005</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>2616.4299999999998</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>82.55</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>62.91</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>0.52506003999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>705.52</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>748.31</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>2377.6</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>78.09</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>50.3</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>0.69049506000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>712.88</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>701.49</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>2422.56</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>75.55</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>55.16</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>0.56140915999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>706.55</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>732.54</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>2397.77</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>77.7</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>51.81</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>0.62085374999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>731.84</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>663.02</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>2429.4299999999998</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>70.61</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>60.27</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>0.55169424</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>726.56</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>749.07</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>2295.44</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>71.83</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>50.23</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <v>0.72304893000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>697.23</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>708.8</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>2489.9</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>81.93</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>54.32</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <v>0.54488961999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>698.38</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>743.59</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>2424.86</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>81.290000000000006</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>50.74</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <v>0.64193677000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>722.41</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>654.33000000000004</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>2477.38</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>72.86</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>61.63</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <v>0.55435942999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>706.04</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>653.29</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>2544.36</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>77.89</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>61.8</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>0.53440182999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>706.76</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>686.73</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>2475.35</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>77.62</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>56.97</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <v>0.53154442000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>703.35</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>637.73</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>2592.2600000000002</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>78.959999999999994</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>64.53</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <v>0.56424830000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>715.39</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>737.94</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>2351.92</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>74.790000000000006</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>51.28</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
         <v>0.65169942999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>696.98</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>664.28</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>2573.8200000000002</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>82.08</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <v>60.08</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <v>0.50742390999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>713.04</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>635.89</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>2552.7199999999998</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>75.5</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>64.88</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
         <v>0.58229849</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>703.06</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>708.35</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>2455.36</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>79.08</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>54.37</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <v>0.55898139000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>693.28</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>641.84</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>2653.6</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>84.71</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>63.77</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <v>0.51934248999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>693.99</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>719.21</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>2498.9499999999998</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>84.11</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>53.18</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
         <v>0.54344466000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>704.67</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>683.19</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>2491.96</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>78.42</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>57.43</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <v>0.52480357</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>728.25</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>661.18</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>2444.1999999999998</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <v>71.430000000000007</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>60.55</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
         <v>0.55301999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>720.65</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>642.39</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>2509.42</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>73.319999999999993</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <v>63.67</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="1">
         <v>0.57677286000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>704.27</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>655.39</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>2548.62</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>78.58</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <v>61.46</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="1">
         <v>0.53145823000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>708.09</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>638.37</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>2567.87</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <v>77.14</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="1">
         <v>64.41</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="1">
         <v>0.56686449000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>708.49</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>638.04999999999995</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>2566.83</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <v>77</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <v>64.47</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="1">
         <v>0.56845857</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>693.6</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>728.85</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>2486.96</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="1">
         <v>84.43</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <v>52.18</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="1">
         <v>0.56843790999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>727.52</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>697.78</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>2377.33</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <v>71.599999999999994</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>55.6</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="1">
         <v>0.57148620000000006</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>695.44</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>691.88</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>2533.36</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="1">
         <v>83.05</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <v>56.32</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="1">
         <v>0.51140982000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>704.88</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <v>649.32000000000005</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>2558.5100000000002</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="1">
         <v>78.34</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <v>62.46</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="1">
         <v>0.53970203000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>696.66</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <v>739.7</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>2443.09</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="1">
         <v>82.27</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="1">
         <v>51.11</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="1">
         <v>0.62052998000000004</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>729.71</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
         <v>659.69</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
         <v>2442.67</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="1">
         <v>71.09</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="1">
         <v>60.78</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="1">
         <v>0.55630075000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>699.13</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <v>660.79</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>2566.34</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="1">
         <v>80.900000000000006</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="1">
         <v>60.61</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="1">
         <v>0.51681591000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="1">
+        <v>709.01</v>
+      </c>
+      <c r="C48" s="1">
+        <v>665.55</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2505.65</v>
+      </c>
+      <c r="E48" s="1">
+        <v>76.819999999999993</v>
+      </c>
+      <c r="F48" s="1">
+        <v>59.89</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.52764898999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" s="1">
+        <v>731.66</v>
+      </c>
+      <c r="C49" s="1">
+        <v>662.36</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2431.3000000000002</v>
+      </c>
+      <c r="E49" s="1">
+        <v>70.650000000000006</v>
+      </c>
+      <c r="F49" s="1">
+        <v>60.37</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0.55255860999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" s="1">
+        <v>718.44</v>
+      </c>
+      <c r="C50" s="1">
+        <v>645.95000000000005</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2509.35</v>
+      </c>
+      <c r="E50" s="1">
+        <v>73.92</v>
+      </c>
+      <c r="F50" s="1">
+        <v>63.04</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0.56364921000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" s="1">
+        <v>724.39</v>
+      </c>
+      <c r="C51" s="1">
+        <v>711.75</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2363.2199999999998</v>
+      </c>
+      <c r="E51" s="1">
+        <v>72.36</v>
+      </c>
+      <c r="F51" s="1">
+        <v>53.99</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0.59478049</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" s="1">
+        <v>693.93</v>
+      </c>
+      <c r="C52" s="1">
+        <v>677.73</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2573.0500000000002</v>
+      </c>
+      <c r="E52" s="1">
+        <v>84.16</v>
+      </c>
+      <c r="F52" s="1">
+        <v>58.16</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0.49152465000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B48">
+      <c r="B53" s="1">
         <v>703.76</v>
       </c>
-      <c r="C48">
+      <c r="C53" s="1">
         <v>647.16</v>
       </c>
-      <c r="D48">
+      <c r="D53" s="1">
         <v>2568.87</v>
       </c>
-      <c r="E48">
+      <c r="E53" s="1">
         <v>78.790000000000006</v>
       </c>
-      <c r="F48">
+      <c r="F53" s="1">
         <v>62.83</v>
       </c>
-      <c r="G48">
+      <c r="G53" s="1">
         <v>0.54281999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B49">
+      <c r="B54" s="1">
         <v>700.24</v>
       </c>
-      <c r="C49">
+      <c r="C54" s="1">
         <v>720.72</v>
       </c>
-      <c r="D49">
+      <c r="D54" s="1">
         <v>2450.27</v>
       </c>
-      <c r="E49">
+      <c r="E54" s="1">
         <v>80.349999999999994</v>
       </c>
-      <c r="F49">
+      <c r="F54" s="1">
         <v>53.02</v>
       </c>
-      <c r="G49">
+      <c r="G54" s="1">
         <v>0.57530000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B50">
+      <c r="B55" s="1">
         <v>696.08</v>
       </c>
-      <c r="C50">
+      <c r="C55" s="1">
         <v>645.6</v>
       </c>
-      <c r="D50">
+      <c r="D55" s="1">
         <v>2619.81</v>
       </c>
-      <c r="E50">
+      <c r="E55" s="1">
         <v>82.63</v>
       </c>
-      <c r="F50">
+      <c r="F55" s="1">
         <v>63.1</v>
       </c>
-      <c r="G50">
+      <c r="G55" s="1">
         <v>0.52761000000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B51">
+      <c r="B56" s="1">
         <v>709.04</v>
       </c>
-      <c r="C51">
+      <c r="C56" s="1">
         <v>736.29</v>
       </c>
-      <c r="D51">
+      <c r="D56" s="1">
         <v>2380.4499999999998</v>
       </c>
-      <c r="E51">
+      <c r="E56" s="1">
         <v>76.81</v>
       </c>
-      <c r="F51">
+      <c r="F56" s="1">
         <v>51.44</v>
       </c>
-      <c r="G51">
+      <c r="G56" s="1">
         <v>0.63507999999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B52">
+      <c r="B57" s="1">
         <v>722.26</v>
       </c>
-      <c r="C52">
+      <c r="C57" s="1">
         <v>681</v>
       </c>
-      <c r="D52">
+      <c r="D57" s="1">
         <v>2425.13</v>
       </c>
-      <c r="E52">
+      <c r="E57" s="1">
         <v>72.900000000000006</v>
       </c>
-      <c r="F52">
+      <c r="F57" s="1">
         <v>57.72</v>
       </c>
-      <c r="G52">
+      <c r="G57" s="1">
         <v>0.54620000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B53">
+      <c r="B58" s="1">
         <v>696.71</v>
       </c>
-      <c r="C53">
+      <c r="C58" s="1">
         <v>658.54</v>
       </c>
-      <c r="D53">
+      <c r="D58" s="1">
         <v>2587.46</v>
       </c>
-      <c r="E53">
+      <c r="E58" s="1">
         <v>82.24</v>
       </c>
-      <c r="F53">
+      <c r="F58" s="1">
         <v>60.96</v>
       </c>
-      <c r="G53">
+      <c r="G58" s="1">
         <v>0.51171</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
         <v>57</v>
       </c>
-      <c r="B54">
+      <c r="B59" s="1">
         <v>717.05</v>
       </c>
-      <c r="C54">
+      <c r="C59" s="1">
         <v>718.28</v>
       </c>
-      <c r="D54">
+      <c r="D59" s="1">
         <v>2377.8200000000002</v>
       </c>
-      <c r="E54">
+      <c r="E59" s="1">
         <v>74.31</v>
       </c>
-      <c r="F54">
+      <c r="F59" s="1">
         <v>53.28</v>
       </c>
-      <c r="G54">
+      <c r="G59" s="1">
         <v>0.59201000000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
         <v>58</v>
       </c>
-      <c r="B55">
+      <c r="B60" s="1">
         <v>703.54</v>
       </c>
-      <c r="C55">
+      <c r="C60" s="1">
         <v>643.62</v>
       </c>
-      <c r="D55">
+      <c r="D60" s="1">
         <v>2577.8200000000002</v>
       </c>
-      <c r="E55">
+      <c r="E60" s="1">
         <v>78.88</v>
       </c>
-      <c r="F55">
+      <c r="F60" s="1">
         <v>63.45</v>
       </c>
-      <c r="G55">
+      <c r="G60" s="1">
         <v>0.55096000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B56">
+      <c r="B61" s="1">
         <v>730.9</v>
       </c>
-      <c r="C56">
+      <c r="C61" s="1">
         <v>730.63</v>
       </c>
-      <c r="D56">
+      <c r="D61" s="1">
         <v>2311.2399999999998</v>
       </c>
-      <c r="E56">
+      <c r="E61" s="1">
         <v>70.819999999999993</v>
       </c>
-      <c r="F56">
+      <c r="F61" s="1">
         <v>52</v>
       </c>
-      <c r="G56">
+      <c r="G61" s="1">
         <v>0.64253000000000005</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B57">
+      <c r="B62" s="1">
         <v>712.91</v>
       </c>
-      <c r="C57">
+      <c r="C62" s="1">
         <v>726.01</v>
       </c>
-      <c r="D57">
+      <c r="D62" s="1">
         <v>2380.91</v>
       </c>
-      <c r="E57">
+      <c r="E62" s="1">
         <v>75.540000000000006</v>
       </c>
-      <c r="F57">
+      <c r="F62" s="1">
         <v>52.47</v>
       </c>
-      <c r="G57">
+      <c r="G62" s="1">
         <v>0.60855000000000004</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B58">
+      <c r="B63" s="1">
         <v>711.03</v>
       </c>
-      <c r="C58">
+      <c r="C63" s="1">
         <v>711.66</v>
       </c>
-      <c r="D58">
+      <c r="D63" s="1">
         <v>2412.56</v>
       </c>
-      <c r="E58">
+      <c r="E63" s="1">
         <v>76.14</v>
       </c>
-      <c r="F58">
+      <c r="F63" s="1">
         <v>54</v>
       </c>
-      <c r="G58">
+      <c r="G63" s="1">
         <v>0.57737000000000005</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B59">
+      <c r="B64" s="1">
         <v>698.92</v>
       </c>
-      <c r="C59">
+      <c r="C64" s="1">
         <v>717.9</v>
       </c>
-      <c r="D59">
+      <c r="D64" s="1">
         <v>2463.14</v>
       </c>
-      <c r="E59">
+      <c r="E64" s="1">
         <v>81.010000000000005</v>
       </c>
-      <c r="F59">
+      <c r="F64" s="1">
         <v>53.32</v>
       </c>
-      <c r="G59">
+      <c r="G64" s="1">
         <v>0.56345999999999996</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B60">
+      <c r="B65" s="1">
         <v>733.94</v>
       </c>
-      <c r="C60">
+      <c r="C65" s="1">
         <v>685.34</v>
       </c>
-      <c r="D60">
+      <c r="D65" s="1">
         <v>2380.23</v>
       </c>
-      <c r="E60">
+      <c r="E65" s="1">
         <v>70.150000000000006</v>
       </c>
-      <c r="F60">
+      <c r="F65" s="1">
         <v>57.15</v>
       </c>
-      <c r="G60">
+      <c r="G65" s="1">
         <v>0.55818000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B61">
+      <c r="B66" s="1">
         <v>701.02</v>
       </c>
-      <c r="C61">
+      <c r="C66" s="1">
         <v>720.35</v>
       </c>
-      <c r="D61">
+      <c r="D66" s="1">
         <v>2446.31</v>
       </c>
-      <c r="E61">
+      <c r="E66" s="1">
         <v>79.98</v>
       </c>
-      <c r="F61">
+      <c r="F66" s="1">
         <v>53.06</v>
       </c>
-      <c r="G61">
+      <c r="G66" s="1">
         <v>0.57562000000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B62">
+      <c r="B67" s="1">
         <v>708.8</v>
       </c>
-      <c r="C62">
+      <c r="C67" s="1">
         <v>720.06</v>
       </c>
-      <c r="D62">
+      <c r="D67" s="1">
         <v>2407.98</v>
       </c>
-      <c r="E62">
+      <c r="E67" s="1">
         <v>76.89</v>
       </c>
-      <c r="F62">
+      <c r="F67" s="1">
         <v>53.09</v>
       </c>
-      <c r="G62">
+      <c r="G67" s="1">
         <v>0.58557000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63">
+    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B63">
+      <c r="B68" s="1">
         <v>718.98</v>
       </c>
-      <c r="C63">
+      <c r="C68" s="1">
         <v>644.47</v>
       </c>
-      <c r="D63">
+      <c r="D68" s="1">
         <v>2510.67</v>
       </c>
-      <c r="E63">
+      <c r="E68" s="1">
         <v>73.77</v>
       </c>
-      <c r="F63">
+      <c r="F68" s="1">
         <v>63.3</v>
       </c>
-      <c r="G63">
+      <c r="G68" s="1">
         <v>0.56845000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B64">
+      <c r="B69" s="1">
         <v>693.04</v>
       </c>
-      <c r="C64">
+      <c r="C69" s="1">
         <v>728.45</v>
       </c>
-      <c r="D64">
+      <c r="D69" s="1">
         <v>2493.6799999999998</v>
       </c>
-      <c r="E64">
+      <c r="E69" s="1">
         <v>84.93</v>
       </c>
-      <c r="F64">
+      <c r="F69" s="1">
         <v>52.22</v>
       </c>
-      <c r="G64">
+      <c r="G69" s="1">
         <v>0.56301000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65">
+    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
         <v>68</v>
       </c>
-      <c r="B65">
+      <c r="B70" s="1">
         <v>697.6</v>
       </c>
-      <c r="C65">
+      <c r="C70" s="1">
         <v>748.74</v>
       </c>
-      <c r="D65">
+      <c r="D70" s="1">
         <v>2422.06</v>
       </c>
-      <c r="E65">
+      <c r="E70" s="1">
         <v>81.72</v>
       </c>
-      <c r="F65">
+      <c r="F70" s="1">
         <v>50.26</v>
       </c>
-      <c r="G65">
+      <c r="G70" s="1">
         <v>0.67218</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66">
+    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B66">
+      <c r="B71" s="1">
         <v>720.92</v>
       </c>
-      <c r="C66">
+      <c r="C71" s="1">
         <v>710.31</v>
       </c>
-      <c r="D66">
+      <c r="D71" s="1">
         <v>2377.42</v>
       </c>
-      <c r="E66">
+      <c r="E71" s="1">
         <v>73.25</v>
       </c>
-      <c r="F66">
+      <c r="F71" s="1">
         <v>54.15</v>
       </c>
-      <c r="G66">
+      <c r="G71" s="1">
         <v>0.58660999999999996</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67">
+    <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B67">
+      <c r="B72" s="1">
         <v>697.13</v>
       </c>
-      <c r="C67">
+      <c r="C72" s="1">
         <v>707.91</v>
       </c>
-      <c r="D67">
+      <c r="D72" s="1">
         <v>2492.16</v>
       </c>
-      <c r="E67">
+      <c r="E72" s="1">
         <v>81.99</v>
       </c>
-      <c r="F67">
+      <c r="F72" s="1">
         <v>54.42</v>
       </c>
-      <c r="G67">
+      <c r="G72" s="1">
         <v>0.54318999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68">
+    <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
         <v>71</v>
       </c>
-      <c r="B68">
+      <c r="B73" s="1">
         <v>705.34</v>
       </c>
-      <c r="C68">
+      <c r="C73" s="1">
         <v>717.25</v>
       </c>
-      <c r="D68">
+      <c r="D73" s="1">
         <v>2428.73</v>
       </c>
-      <c r="E68">
+      <c r="E73" s="1">
         <v>78.16</v>
       </c>
-      <c r="F68">
+      <c r="F73" s="1">
         <v>53.39</v>
       </c>
-      <c r="G68">
+      <c r="G73" s="1">
         <v>0.57399999999999995</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69">
+    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
         <v>72</v>
       </c>
-      <c r="B69">
+      <c r="B74" s="1">
         <v>701.82</v>
       </c>
-      <c r="C69">
+      <c r="C74" s="1">
         <v>636.57000000000005</v>
       </c>
-      <c r="D69">
+      <c r="D74" s="1">
         <v>2603.1999999999998</v>
       </c>
-      <c r="E69">
+      <c r="E74" s="1">
         <v>79.62</v>
       </c>
-      <c r="F69">
+      <c r="F74" s="1">
         <v>64.75</v>
       </c>
-      <c r="G69">
+      <c r="G74" s="1">
         <v>0.56501000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70">
+    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
         <v>73</v>
       </c>
-      <c r="B70">
+      <c r="B75" s="1">
         <v>698.53</v>
       </c>
-      <c r="C70">
+      <c r="C75" s="1">
         <v>685.03</v>
       </c>
-      <c r="D70">
+      <c r="D75" s="1">
         <v>2523.2600000000002</v>
       </c>
-      <c r="E70">
+      <c r="E75" s="1">
         <v>81.209999999999994</v>
       </c>
-      <c r="F70">
+      <c r="F75" s="1">
         <v>57.19</v>
       </c>
-      <c r="G70">
+      <c r="G75" s="1">
         <v>0.51698999999999995</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71">
+    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
         <v>74</v>
       </c>
-      <c r="B71">
+      <c r="B76" s="1">
         <v>696.32</v>
       </c>
-      <c r="C71">
+      <c r="C76" s="1">
         <v>651.59</v>
       </c>
-      <c r="D71">
+      <c r="D76" s="1">
         <v>2604.9699999999998</v>
       </c>
-      <c r="E71">
+      <c r="E76" s="1">
         <v>82.48</v>
       </c>
-      <c r="F71">
+      <c r="F76" s="1">
         <v>62.08</v>
       </c>
-      <c r="G71">
+      <c r="G76" s="1">
         <v>0.51807000000000003</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72">
+    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
         <v>75</v>
       </c>
-      <c r="B72">
+      <c r="B77" s="1">
         <v>718.22</v>
       </c>
-      <c r="C72">
+      <c r="C77" s="1">
         <v>708.44</v>
       </c>
-      <c r="D72">
+      <c r="D77" s="1">
         <v>2390.1799999999998</v>
       </c>
-      <c r="E72">
+      <c r="E77" s="1">
         <v>73.98</v>
       </c>
-      <c r="F72">
+      <c r="F77" s="1">
         <v>54.36</v>
       </c>
-      <c r="G72">
+      <c r="G77" s="1">
         <v>0.57925000000000004</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73">
+    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B73">
+      <c r="B78" s="1">
         <v>723.12</v>
       </c>
-      <c r="C73">
+      <c r="C78" s="1">
         <v>742</v>
       </c>
-      <c r="D73">
+      <c r="D78" s="1">
         <v>2317.85</v>
       </c>
-      <c r="E73">
+      <c r="E78" s="1">
         <v>72.680000000000007</v>
       </c>
-      <c r="F73">
+      <c r="F78" s="1">
         <v>50.89</v>
       </c>
-      <c r="G73">
+      <c r="G78" s="1">
         <v>0.68172999999999995</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74">
+    <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B74">
+      <c r="B79" s="1">
         <v>723.83</v>
       </c>
-      <c r="C74">
+      <c r="C79" s="1">
         <v>647.27</v>
       </c>
-      <c r="D74">
+      <c r="D79" s="1">
         <v>2487.77</v>
       </c>
-      <c r="E74">
+      <c r="E79" s="1">
         <v>72.5</v>
       </c>
-      <c r="F74">
+      <c r="F79" s="1">
         <v>62.81</v>
       </c>
-      <c r="G74">
+      <c r="G79" s="1">
         <v>0.56933</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75">
+    <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B75">
+      <c r="B80" s="1">
         <v>705.34</v>
       </c>
-      <c r="C75">
+      <c r="C80" s="1">
         <v>720.16</v>
       </c>
-      <c r="D75">
+      <c r="D80" s="1">
         <v>2423.88</v>
       </c>
-      <c r="E75">
+      <c r="E80" s="1">
         <v>78.16</v>
       </c>
-      <c r="F75">
+      <c r="F80" s="1">
         <v>53.08</v>
       </c>
-      <c r="G75">
+      <c r="G80" s="1">
         <v>0.58235999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76">
+    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B76">
+      <c r="B81" s="1">
         <v>706.58</v>
       </c>
-      <c r="C76">
+      <c r="C81" s="1">
         <v>670.7</v>
       </c>
-      <c r="D76">
+      <c r="D81" s="1">
         <v>2506.52</v>
       </c>
-      <c r="E76">
+      <c r="E81" s="1">
         <v>77.69</v>
       </c>
-      <c r="F76">
+      <c r="F81" s="1">
         <v>59.14</v>
       </c>
-      <c r="G76">
+      <c r="G81" s="1">
         <v>0.52276999999999996</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77">
+    <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B77">
+      <c r="B82" s="1">
         <v>722.26</v>
       </c>
-      <c r="C77">
+      <c r="C82" s="1">
         <v>677.8</v>
       </c>
-      <c r="D77">
+      <c r="D82" s="1">
         <v>2431.15</v>
       </c>
-      <c r="E77">
+      <c r="E82" s="1">
         <v>72.900000000000006</v>
       </c>
-      <c r="F77">
+      <c r="F82" s="1">
         <v>58.15</v>
       </c>
-      <c r="G77">
+      <c r="G82" s="1">
         <v>0.54313</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78">
+    <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
         <v>81</v>
       </c>
-      <c r="B78">
+      <c r="B83" s="1">
         <v>706.17</v>
       </c>
-      <c r="C78">
+      <c r="C83" s="1">
         <v>716.6</v>
       </c>
-      <c r="D78">
+      <c r="D83" s="1">
         <v>2425.79</v>
       </c>
-      <c r="E78">
+      <c r="E83" s="1">
         <v>77.84</v>
       </c>
-      <c r="F78">
+      <c r="F83" s="1">
         <v>53.46</v>
       </c>
-      <c r="G78">
+      <c r="G83" s="1">
         <v>0.57533999999999996</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79">
+    <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
         <v>82</v>
       </c>
-      <c r="B79">
+      <c r="B84" s="1">
         <v>695.01</v>
       </c>
-      <c r="C79">
+      <c r="C84" s="1">
         <v>666.43</v>
       </c>
-      <c r="D79">
+      <c r="D84" s="1">
         <v>2585.08</v>
       </c>
-      <c r="E79">
+      <c r="E84" s="1">
         <v>83.35</v>
       </c>
-      <c r="F79">
+      <c r="F84" s="1">
         <v>59.76</v>
       </c>
-      <c r="G79">
+      <c r="G84" s="1">
         <v>0.49913000000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80">
+    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
         <v>83</v>
       </c>
-      <c r="B80">
+      <c r="B85" s="1">
         <v>714.25</v>
       </c>
-      <c r="C80">
+      <c r="C85" s="1">
         <v>651.89</v>
       </c>
-      <c r="D80">
+      <c r="D85" s="1">
         <v>2512.16</v>
       </c>
-      <c r="E80">
+      <c r="E85" s="1">
         <v>75.13</v>
       </c>
-      <c r="F80">
+      <c r="F85" s="1">
         <v>62.03</v>
       </c>
-      <c r="G80">
+      <c r="G85" s="1">
         <v>0.54994200000000004</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81">
+    <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
         <v>84</v>
       </c>
-      <c r="B81">
+      <c r="B86" s="1">
         <v>712.4</v>
       </c>
-      <c r="C81">
+      <c r="C86" s="1">
         <v>743.06</v>
       </c>
-      <c r="D81">
+      <c r="D86" s="1">
         <v>2355.5</v>
       </c>
-      <c r="E81">
+      <c r="E86" s="1">
         <v>75.7</v>
       </c>
-      <c r="F81">
+      <c r="F86" s="1">
         <v>50.79</v>
       </c>
-      <c r="G81">
+      <c r="G86" s="1">
         <v>0.66925000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82">
+    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
         <v>85</v>
       </c>
-      <c r="B82">
+      <c r="B87" s="1">
         <v>706.55</v>
       </c>
-      <c r="C82">
+      <c r="C87" s="1">
         <v>655.89</v>
       </c>
-      <c r="D82">
+      <c r="D87" s="1">
         <v>2536.5100000000002</v>
       </c>
-      <c r="E82">
+      <c r="E87" s="1">
         <v>77.7</v>
       </c>
-      <c r="F82">
+      <c r="F87" s="1">
         <v>61.38</v>
       </c>
-      <c r="G82">
+      <c r="G87" s="1">
         <v>0.53271999999999997</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83">
+    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
         <v>86</v>
       </c>
-      <c r="B83">
+      <c r="B88" s="1">
         <v>713.33</v>
       </c>
-      <c r="C83">
+      <c r="C88" s="1">
         <v>727.86</v>
       </c>
-      <c r="D83">
+      <c r="D88" s="1">
         <v>2376.1999999999998</v>
       </c>
-      <c r="E83">
+      <c r="E88" s="1">
         <v>75.41</v>
       </c>
-      <c r="F83">
+      <c r="F88" s="1">
         <v>52.28</v>
       </c>
-      <c r="G83">
+      <c r="G88" s="1">
         <v>0.61428000000000005</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84">
+    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
         <v>87</v>
       </c>
-      <c r="B84">
+      <c r="B89" s="1">
         <v>722.57</v>
       </c>
-      <c r="C84">
+      <c r="C89" s="1">
         <v>654.64</v>
       </c>
-      <c r="D84">
+      <c r="D89" s="1">
         <v>2476.1999999999998</v>
       </c>
-      <c r="E84">
+      <c r="E89" s="1">
         <v>72.819999999999993</v>
       </c>
-      <c r="F84">
+      <c r="F89" s="1">
         <v>61.58</v>
       </c>
-      <c r="G84">
+      <c r="G89" s="1">
         <v>0.55352999999999997</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85">
+    <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
         <v>88</v>
       </c>
-      <c r="B85">
+      <c r="B90" s="1">
         <v>696.16</v>
       </c>
-      <c r="C85">
+      <c r="C90" s="1">
         <v>693.66</v>
       </c>
-      <c r="D85">
+      <c r="D90" s="1">
         <v>2524.41</v>
       </c>
-      <c r="E85">
+      <c r="E90" s="1">
         <v>82.58</v>
       </c>
-      <c r="F85">
+      <c r="F90" s="1">
         <v>56.1</v>
       </c>
-      <c r="G85">
+      <c r="G90" s="1">
         <v>0.51719999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86">
+    <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
         <v>89</v>
       </c>
-      <c r="B86">
+      <c r="B91" s="1">
         <v>734.4</v>
       </c>
-      <c r="C86">
+      <c r="C91" s="1">
         <v>637.62</v>
       </c>
-      <c r="D86">
+      <c r="D91" s="1">
         <v>2476.62</v>
       </c>
-      <c r="E86">
+      <c r="E91" s="1">
         <v>70.05</v>
       </c>
-      <c r="F86">
+      <c r="F91" s="1">
         <v>64.55</v>
       </c>
-      <c r="G86">
+      <c r="G91" s="1">
         <v>0.59862000000000004</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87">
+    <row r="92" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
         <v>90</v>
       </c>
-      <c r="B87">
+      <c r="B92" s="1">
         <v>724.88</v>
       </c>
-      <c r="C87">
+      <c r="C92" s="1">
         <v>738.56</v>
       </c>
-      <c r="D87">
+      <c r="D92" s="1">
         <v>2317.5</v>
       </c>
-      <c r="E87">
+      <c r="E92" s="1">
         <v>72.239999999999995</v>
       </c>
-      <c r="F87">
+      <c r="F92" s="1">
         <v>51.22</v>
       </c>
-      <c r="G87">
+      <c r="G92" s="1">
         <v>0.66757</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88">
+    <row r="93" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
         <v>91</v>
       </c>
-      <c r="B88">
+      <c r="B93" s="1">
         <v>712.66</v>
       </c>
-      <c r="C88">
+      <c r="C93" s="1">
         <v>649.15</v>
       </c>
-      <c r="D88">
+      <c r="D93" s="1">
         <v>2524.36</v>
       </c>
-      <c r="E88">
+      <c r="E93" s="1">
         <v>75.62</v>
       </c>
-      <c r="F88">
+      <c r="F93" s="1">
         <v>62.49</v>
       </c>
-      <c r="G88">
+      <c r="G93" s="1">
         <v>0.54995000000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89">
+    <row r="94" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
         <v>92</v>
       </c>
-      <c r="B89">
+      <c r="B94" s="1">
         <v>705.21</v>
       </c>
-      <c r="C89">
+      <c r="C94" s="1">
         <v>723.2</v>
       </c>
-      <c r="D89">
+      <c r="D94" s="1">
         <v>2419.4499999999998</v>
       </c>
-      <c r="E89">
+      <c r="E94" s="1">
         <v>78.209999999999994</v>
       </c>
-      <c r="F89">
+      <c r="F94" s="1">
         <v>52.76</v>
       </c>
-      <c r="G89">
+      <c r="G94" s="1">
         <v>0.58938999999999997</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90">
+    <row r="95" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
         <v>93</v>
       </c>
-      <c r="B90">
+      <c r="B95" s="1">
         <v>693.97</v>
       </c>
-      <c r="C90">
+      <c r="C95" s="1">
         <v>660.27</v>
       </c>
-      <c r="D90">
+      <c r="D95" s="1">
         <v>2607</v>
       </c>
-      <c r="E90">
+      <c r="E95" s="1">
         <v>84.13</v>
       </c>
-      <c r="F90">
+      <c r="F95" s="1">
         <v>60.69</v>
       </c>
-      <c r="G90">
+      <c r="G95" s="1">
         <v>0.49629000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91">
+    <row r="96" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
         <v>94</v>
       </c>
-      <c r="B91">
+      <c r="B96" s="1">
         <v>696.43</v>
       </c>
-      <c r="C91">
+      <c r="C96" s="1">
         <v>644.47</v>
       </c>
-      <c r="D91">
+      <c r="D96" s="1">
         <v>2619.64</v>
       </c>
-      <c r="E91">
+      <c r="E96" s="1">
         <v>82.41</v>
       </c>
-      <c r="F91">
+      <c r="F96" s="1">
         <v>63.3</v>
       </c>
-      <c r="G91">
+      <c r="G96" s="1">
         <v>0.53081</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92">
+    <row r="97" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
         <v>95</v>
       </c>
-      <c r="B92">
+      <c r="B97" s="1">
         <v>696.73</v>
       </c>
-      <c r="C92">
+      <c r="C97" s="1">
         <v>664.15</v>
       </c>
-      <c r="D92">
+      <c r="D97" s="1">
         <v>2575.9299999999998</v>
       </c>
-      <c r="E92">
+      <c r="E97" s="1">
         <v>82.23</v>
       </c>
-      <c r="F92">
+      <c r="F97" s="1">
         <v>60.1</v>
       </c>
-      <c r="G92">
+      <c r="G97" s="1">
         <v>0.50661999999999996</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93">
+    <row r="98" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
         <v>96</v>
       </c>
-      <c r="B93">
-        <v>705.21</v>
-      </c>
-      <c r="C93">
-        <v>687.67</v>
-      </c>
-      <c r="D93">
-        <v>2481.06</v>
-      </c>
-      <c r="E93">
-        <v>78.209999999999994</v>
-      </c>
-      <c r="F93">
-        <v>56.85</v>
-      </c>
-      <c r="G93">
-        <v>0.52942</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94">
+      <c r="B98" s="1">
+        <v>706.46</v>
+      </c>
+      <c r="C98" s="1">
+        <v>677.49</v>
+      </c>
+      <c r="D98" s="1">
+        <v>2493.9699999999998</v>
+      </c>
+      <c r="E98" s="1">
+        <v>77.73</v>
+      </c>
+      <c r="F98" s="1">
+        <v>58.19</v>
+      </c>
+      <c r="G98" s="2">
+        <v>0.52873999999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
         <v>97</v>
       </c>
-      <c r="B94">
-        <v>711.16</v>
-      </c>
-      <c r="C94">
-        <v>731.43</v>
-      </c>
-      <c r="D94">
-        <v>2379.2399999999998</v>
-      </c>
-      <c r="E94">
-        <v>76.099999999999994</v>
-      </c>
-      <c r="F94">
-        <v>51.92</v>
-      </c>
-      <c r="G94">
-        <v>0.62468000000000001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95">
+      <c r="B99" s="1">
+        <v>703.64</v>
+      </c>
+      <c r="C99" s="1">
+        <v>715.86</v>
+      </c>
+      <c r="D99" s="1">
+        <v>2439.6</v>
+      </c>
+      <c r="E99" s="1">
+        <v>78.84</v>
+      </c>
+      <c r="F99" s="1">
+        <v>53.54</v>
+      </c>
+      <c r="G99" s="2">
+        <v>0.57069999999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
         <v>98</v>
       </c>
-      <c r="B95">
-        <v>694.95</v>
-      </c>
-      <c r="C95">
-        <v>676.85</v>
-      </c>
-      <c r="D95">
-        <v>2565.33</v>
-      </c>
-      <c r="E95">
-        <v>83.39</v>
-      </c>
-      <c r="F95">
-        <v>58.28</v>
-      </c>
-      <c r="G95">
-        <v>0.49682999999999999</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96">
+      <c r="B100" s="1">
+        <v>694.87</v>
+      </c>
+      <c r="C100" s="1">
+        <v>706.94</v>
+      </c>
+      <c r="D100" s="1">
+        <v>2511.71</v>
+      </c>
+      <c r="E100" s="1">
+        <v>83.45</v>
+      </c>
+      <c r="F100" s="1">
+        <v>54.53</v>
+      </c>
+      <c r="G100" s="2">
+        <v>0.53220000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
         <v>99</v>
       </c>
-      <c r="B96">
-        <v>693.2</v>
-      </c>
-      <c r="C96">
-        <v>641.55999999999995</v>
-      </c>
-      <c r="D96">
-        <v>2655.07</v>
-      </c>
-      <c r="E96">
-        <v>84.78</v>
-      </c>
-      <c r="F96">
-        <v>63.82</v>
-      </c>
-      <c r="G96">
-        <v>0.51873000000000002</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97">
+      <c r="B101" s="1">
+        <v>703.88</v>
+      </c>
+      <c r="C101" s="1">
+        <v>724.55</v>
+      </c>
+      <c r="D101" s="1">
+        <v>2423.88</v>
+      </c>
+      <c r="E101" s="1">
+        <v>78.739999999999995</v>
+      </c>
+      <c r="F101" s="1">
+        <v>52.62</v>
+      </c>
+      <c r="G101" s="2">
+        <v>0.59033000000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="1">
         <v>100</v>
       </c>
-      <c r="B97">
-        <v>704.08</v>
-      </c>
-      <c r="C97">
-        <v>738.87</v>
-      </c>
-      <c r="D97">
-        <v>2399.67</v>
-      </c>
-      <c r="E97">
-        <v>78.66</v>
-      </c>
-      <c r="F97">
-        <v>51.19</v>
-      </c>
-      <c r="G97">
-        <v>0.63897000000000004</v>
+      <c r="B102" s="1">
+        <v>710.07</v>
+      </c>
+      <c r="C102" s="1">
+        <v>709.24</v>
+      </c>
+      <c r="D102" s="1">
+        <v>2420.7800000000002</v>
+      </c>
+      <c r="E102" s="1">
+        <v>76.459999999999994</v>
+      </c>
+      <c r="F102" s="1">
+        <v>54.27</v>
+      </c>
+      <c r="G102" s="2">
+        <v>0.57196000000000002</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="B103" s="1">
+        <v>732.02</v>
+      </c>
+      <c r="C103" s="1">
+        <v>680.25</v>
+      </c>
+      <c r="D103" s="1">
+        <v>2395.4</v>
+      </c>
+      <c r="E103" s="1">
+        <v>70.569999999999993</v>
+      </c>
+      <c r="F103" s="1">
+        <v>57.82</v>
+      </c>
+      <c r="G103" s="2">
+        <v>0.55212000000000006</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="B104" s="1">
+        <v>695.6</v>
+      </c>
+      <c r="C104" s="1">
+        <v>703.8</v>
+      </c>
+      <c r="D104" s="1">
+        <v>2510.91</v>
+      </c>
+      <c r="E104" s="1">
+        <v>82.94</v>
+      </c>
+      <c r="F104" s="1">
+        <v>54.89</v>
+      </c>
+      <c r="G104" s="2">
+        <v>0.52988999999999997</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="B105" s="1">
+        <v>696.64</v>
+      </c>
+      <c r="C105" s="1">
+        <v>703.12</v>
+      </c>
+      <c r="D105" s="1">
+        <v>2504.02</v>
+      </c>
+      <c r="E105" s="1">
+        <v>82.28</v>
+      </c>
+      <c r="F105" s="1">
+        <v>54.97</v>
+      </c>
+      <c r="G105" s="2">
+        <v>0.53502000000000005</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106" s="1">
+        <v>721.8</v>
+      </c>
+      <c r="C106" s="1">
+        <v>688.46</v>
+      </c>
+      <c r="D106" s="1">
+        <v>2412.9299999999998</v>
+      </c>
+      <c r="E106" s="1">
+        <v>73.02</v>
+      </c>
+      <c r="F106" s="1">
+        <v>56.75</v>
+      </c>
+      <c r="G106" s="2">
+        <v>0.55225999999999997</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107" s="1">
+        <v>704</v>
+      </c>
+      <c r="C107" s="1">
+        <v>675.54</v>
+      </c>
+      <c r="D107" s="1">
+        <v>2509.7600000000002</v>
+      </c>
+      <c r="E107" s="1">
+        <v>78.69</v>
+      </c>
+      <c r="F107" s="1">
+        <v>58.46</v>
+      </c>
+      <c r="G107" s="2">
+        <v>0.51859</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108" s="1">
+        <v>734.03</v>
+      </c>
+      <c r="C108" s="1">
+        <v>665.69</v>
+      </c>
+      <c r="D108" s="1">
+        <v>2417.56</v>
+      </c>
+      <c r="E108" s="1">
+        <v>70.13</v>
+      </c>
+      <c r="F108" s="1">
+        <v>59.87</v>
+      </c>
+      <c r="G108" s="2">
+        <v>0.55205000000000004</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109" s="1">
+        <v>707.34</v>
+      </c>
+      <c r="C109" s="1">
+        <v>729.24</v>
+      </c>
+      <c r="D109" s="1">
+        <v>2399.4499999999998</v>
+      </c>
+      <c r="E109" s="1">
+        <v>77.41</v>
+      </c>
+      <c r="F109" s="1">
+        <v>52.14</v>
+      </c>
+      <c r="G109" s="2">
+        <v>0.61107999999999996</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110" s="1">
+        <v>723.39</v>
+      </c>
+      <c r="C110" s="1">
+        <v>721.39</v>
+      </c>
+      <c r="D110" s="1">
+        <v>2350.35</v>
+      </c>
+      <c r="E110" s="1">
+        <v>72.61</v>
+      </c>
+      <c r="F110" s="1">
+        <v>52.95</v>
+      </c>
+      <c r="G110" s="2">
+        <v>0.61087000000000002</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111" s="1">
+        <v>698.78</v>
+      </c>
+      <c r="C111" s="1">
+        <v>645.95000000000005</v>
+      </c>
+      <c r="D111" s="1">
+        <v>2599.9899999999998</v>
+      </c>
+      <c r="E111" s="1">
+        <v>81.08</v>
+      </c>
+      <c r="F111" s="1">
+        <v>63.04</v>
+      </c>
+      <c r="G111" s="2">
+        <v>0.53561000000000003</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="B112" s="1">
+        <v>731.48</v>
+      </c>
+      <c r="C112" s="1">
+        <v>704.15</v>
+      </c>
+      <c r="D112" s="1">
+        <v>2353.92</v>
+      </c>
+      <c r="E112" s="1">
+        <v>70.69</v>
+      </c>
+      <c r="F112" s="1">
+        <v>54.85</v>
+      </c>
+      <c r="G112" s="2">
+        <v>0.58311000000000002</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>111</v>
+      </c>
+      <c r="B113" s="1">
+        <v>709.12</v>
+      </c>
+      <c r="C113" s="1">
+        <v>671.4</v>
+      </c>
+      <c r="D113" s="1">
+        <v>2493.63</v>
+      </c>
+      <c r="E113" s="1">
+        <v>76.78</v>
+      </c>
+      <c r="F113" s="1">
+        <v>59.04</v>
+      </c>
+      <c r="G113" s="2">
+        <v>0.52569999999999995</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>112</v>
+      </c>
+      <c r="B114" s="1">
+        <v>710.24</v>
+      </c>
+      <c r="C114" s="1">
+        <v>651.95000000000005</v>
+      </c>
+      <c r="D114" s="1">
+        <v>2528.31</v>
+      </c>
+      <c r="E114" s="1">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="F114" s="1">
+        <v>62.02</v>
+      </c>
+      <c r="G114" s="2">
+        <v>0.54318</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>113</v>
+      </c>
+      <c r="B115" s="1">
+        <v>721.83</v>
+      </c>
+      <c r="C115" s="1">
+        <v>681.45</v>
+      </c>
+      <c r="D115" s="1">
+        <v>2425.7399999999998</v>
+      </c>
+      <c r="E115" s="1">
+        <v>73.010000000000005</v>
+      </c>
+      <c r="F115" s="1">
+        <v>57.66</v>
+      </c>
+      <c r="G115" s="2">
+        <v>0.54649000000000003</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>114</v>
+      </c>
+      <c r="B116" s="1">
+        <v>699.58</v>
+      </c>
+      <c r="C116" s="1">
+        <v>651.77</v>
+      </c>
+      <c r="D116" s="1">
+        <v>2582.29</v>
+      </c>
+      <c r="E116" s="1">
+        <v>80.67</v>
+      </c>
+      <c r="F116" s="1">
+        <v>62.05</v>
+      </c>
+      <c r="G116" s="2">
+        <v>0.52907000000000004</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>115</v>
+      </c>
+      <c r="B117" s="1">
+        <v>700.32</v>
+      </c>
+      <c r="C117" s="1">
+        <v>747.23</v>
+      </c>
+      <c r="D117" s="1">
+        <v>2407.02</v>
+      </c>
+      <c r="E117" s="1">
+        <v>80.31</v>
+      </c>
+      <c r="F117" s="1">
+        <v>50.4</v>
+      </c>
+      <c r="G117" s="2">
+        <v>0.66493999999999998</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>116</v>
+      </c>
+      <c r="B118" s="1">
+        <v>704.55</v>
+      </c>
+      <c r="C118" s="1">
+        <v>675.47</v>
+      </c>
+      <c r="D118" s="1">
+        <v>2507.14</v>
+      </c>
+      <c r="E118" s="1">
+        <v>78.47</v>
+      </c>
+      <c r="F118" s="1">
+        <v>58.47</v>
+      </c>
+      <c r="G118" s="2">
+        <v>0.51951000000000003</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>117</v>
+      </c>
+      <c r="B119" s="1">
+        <v>695.8</v>
+      </c>
+      <c r="C119" s="1">
+        <v>718.84</v>
+      </c>
+      <c r="D119" s="1">
+        <v>2483.71</v>
+      </c>
+      <c r="E119" s="1">
+        <v>82.81</v>
+      </c>
+      <c r="F119" s="1">
+        <v>53.22</v>
+      </c>
+      <c r="G119" s="2">
+        <v>0.55335999999999996</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
+        <v>118</v>
+      </c>
+      <c r="B120" s="1">
+        <v>728.67</v>
+      </c>
+      <c r="C120" s="1">
+        <v>700.64</v>
+      </c>
+      <c r="D120" s="1">
+        <v>2368.67</v>
+      </c>
+      <c r="E120" s="1">
+        <v>71.33</v>
+      </c>
+      <c r="F120" s="1">
+        <v>55.26</v>
+      </c>
+      <c r="G120" s="2">
+        <v>0.57657999999999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
+        <v>119</v>
+      </c>
+      <c r="B121" s="1">
+        <v>693.28</v>
+      </c>
+      <c r="C121" s="1">
+        <v>731.33</v>
+      </c>
+      <c r="D121" s="1">
+        <v>2486.3200000000002</v>
+      </c>
+      <c r="E121" s="1">
+        <v>84.71</v>
+      </c>
+      <c r="F121" s="1">
+        <v>51.93</v>
+      </c>
+      <c r="G121" s="2">
+        <v>0.57369000000000003</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
+        <v>120</v>
+      </c>
+      <c r="B122" s="1">
+        <v>716.35</v>
+      </c>
+      <c r="C122" s="1">
+        <v>745.51</v>
+      </c>
+      <c r="D122" s="1">
+        <v>2336.2800000000002</v>
+      </c>
+      <c r="E122" s="1">
+        <v>74.510000000000005</v>
+      </c>
+      <c r="F122" s="1">
+        <v>50.56</v>
+      </c>
+      <c r="G122" s="2">
+        <v>0.68557000000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="1">
+        <v>121</v>
+      </c>
+      <c r="B123" s="1">
+        <v>732.11</v>
+      </c>
+      <c r="C123" s="1">
+        <v>689.56</v>
+      </c>
+      <c r="D123" s="1">
+        <v>2377.92</v>
+      </c>
+      <c r="E123" s="1">
+        <v>70.55</v>
+      </c>
+      <c r="F123" s="1">
+        <v>56.61</v>
+      </c>
+      <c r="G123" s="2">
+        <v>0.56027000000000005</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="1">
+        <v>122</v>
+      </c>
+      <c r="B124" s="1">
+        <v>696.64</v>
+      </c>
+      <c r="C124" s="1">
+        <v>650.63</v>
+      </c>
+      <c r="D124" s="1">
+        <v>2604.5700000000002</v>
+      </c>
+      <c r="E124" s="1">
+        <v>82.28</v>
+      </c>
+      <c r="F124" s="1">
+        <v>62.24</v>
+      </c>
+      <c r="G124" s="2">
+        <v>0.52141000000000004</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="1">
+        <v>123</v>
+      </c>
+      <c r="B125" s="1">
+        <v>716.07</v>
+      </c>
+      <c r="C125" s="1">
+        <v>642.34</v>
+      </c>
+      <c r="D125" s="1">
+        <v>2526.11</v>
+      </c>
+      <c r="E125" s="1">
+        <v>74.59</v>
+      </c>
+      <c r="F125" s="1">
+        <v>63.68</v>
+      </c>
+      <c r="G125" s="2">
+        <v>0.56823999999999997</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="1">
+        <v>124</v>
+      </c>
+      <c r="B126" s="1">
+        <v>721.95</v>
+      </c>
+      <c r="C126" s="1">
+        <v>664.75</v>
+      </c>
+      <c r="D126" s="1">
+        <v>2457.6</v>
+      </c>
+      <c r="E126" s="1">
+        <v>72.98</v>
+      </c>
+      <c r="F126" s="1">
+        <v>60.01</v>
+      </c>
+      <c r="G126" s="2">
+        <v>0.54408886999999995</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="1">
+        <v>125</v>
+      </c>
+      <c r="B127" s="1">
+        <v>697.48</v>
+      </c>
+      <c r="C127" s="1">
+        <v>694.64</v>
+      </c>
+      <c r="D127" s="1">
+        <v>2512.96</v>
+      </c>
+      <c r="E127" s="1">
+        <v>81.790000000000006</v>
+      </c>
+      <c r="F127" s="1">
+        <v>55.98</v>
+      </c>
+      <c r="G127" s="2">
+        <v>0.52329340000000002</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="1">
+        <v>126</v>
+      </c>
+      <c r="B128" s="1">
+        <v>723.12</v>
+      </c>
+      <c r="C128" s="1">
+        <v>691.56</v>
+      </c>
+      <c r="D128" s="1">
+        <v>2402.81</v>
+      </c>
+      <c r="E128" s="1">
+        <v>72.680000000000007</v>
+      </c>
+      <c r="F128" s="1">
+        <v>56.36</v>
+      </c>
+      <c r="G128" s="2">
+        <v>0.55713690999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="1">
+        <v>127</v>
+      </c>
+      <c r="B129" s="1">
+        <v>713.27</v>
+      </c>
+      <c r="C129" s="1">
+        <v>645.89</v>
+      </c>
+      <c r="D129" s="1">
+        <v>2529.04</v>
+      </c>
+      <c r="E129" s="1">
+        <v>75.430000000000007</v>
+      </c>
+      <c r="F129" s="1">
+        <v>63.05</v>
+      </c>
+      <c r="G129" s="2">
+        <v>0.55862650999999997</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="1">
+        <v>128</v>
+      </c>
+      <c r="B130" s="1">
+        <v>717.47</v>
+      </c>
+      <c r="C130" s="1">
+        <v>694.89</v>
+      </c>
+      <c r="D130" s="1">
+        <v>2416.64</v>
+      </c>
+      <c r="E130" s="1">
+        <v>74.19</v>
+      </c>
+      <c r="F130" s="1">
+        <v>55.95</v>
+      </c>
+      <c r="G130" s="2">
+        <v>0.55452018000000003</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="1">
+        <v>129</v>
+      </c>
+      <c r="B131" s="1">
+        <v>700.59</v>
+      </c>
+      <c r="C131" s="1">
+        <v>646.75</v>
+      </c>
+      <c r="D131" s="1">
+        <v>2587.08</v>
+      </c>
+      <c r="E131" s="1">
+        <v>80.180000000000007</v>
+      </c>
+      <c r="F131" s="1">
+        <v>62.9</v>
+      </c>
+      <c r="G131" s="2">
+        <v>0.54071670000000005</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="1">
+        <v>130</v>
+      </c>
+      <c r="B132" s="1">
+        <v>724.51</v>
+      </c>
+      <c r="C132" s="1">
+        <v>717.25</v>
+      </c>
+      <c r="D132" s="1">
+        <v>2353.54</v>
+      </c>
+      <c r="E132" s="1">
+        <v>72.33</v>
+      </c>
+      <c r="F132" s="1">
+        <v>53.39</v>
+      </c>
+      <c r="G132" s="2">
+        <v>0.60040543999999996</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="1">
+        <v>131</v>
+      </c>
+      <c r="B133" s="1">
+        <v>696.25</v>
+      </c>
+      <c r="C133" s="1">
+        <v>644.52</v>
+      </c>
+      <c r="D133" s="1">
+        <v>2620.86</v>
+      </c>
+      <c r="E133" s="1">
+        <v>82.52</v>
+      </c>
+      <c r="F133" s="1">
+        <v>63.29</v>
+      </c>
+      <c r="G133" s="2">
+        <v>0.52944875999999996</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="1">
+        <v>132</v>
+      </c>
+      <c r="B134" s="1">
+        <v>708.89</v>
+      </c>
+      <c r="C134" s="1">
+        <v>655.64</v>
+      </c>
+      <c r="D134" s="1">
+        <v>2526.4</v>
+      </c>
+      <c r="E134" s="1">
+        <v>76.86</v>
+      </c>
+      <c r="F134" s="1">
+        <v>61.42</v>
+      </c>
+      <c r="G134" s="2">
+        <v>0.53536976999999997</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="1">
+        <v>133</v>
+      </c>
+      <c r="B135" s="1">
+        <v>717.61</v>
+      </c>
+      <c r="C135" s="1">
+        <v>663.42</v>
+      </c>
+      <c r="D135" s="1">
+        <v>2475.6</v>
+      </c>
+      <c r="E135" s="1">
+        <v>74.150000000000006</v>
+      </c>
+      <c r="F135" s="1">
+        <v>60.21</v>
+      </c>
+      <c r="G135" s="2">
+        <v>0.53850989000000005</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="1">
+        <v>134</v>
+      </c>
+      <c r="B136" s="1">
+        <v>702.99</v>
+      </c>
+      <c r="C136" s="1">
+        <v>655.95</v>
+      </c>
+      <c r="D136" s="1">
+        <v>2554.08</v>
+      </c>
+      <c r="E136" s="1">
+        <v>79.11</v>
+      </c>
+      <c r="F136" s="1">
+        <v>61.37</v>
+      </c>
+      <c r="G136" s="2">
+        <v>0.52897077999999997</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="B137" s="1">
+        <v>694.07</v>
+      </c>
+      <c r="C137" s="1">
+        <v>653.41</v>
+      </c>
+      <c r="D137" s="1">
+        <v>2620.2800000000002</v>
+      </c>
+      <c r="E137" s="1">
+        <v>84.05</v>
+      </c>
+      <c r="F137" s="1">
+        <v>61.78</v>
+      </c>
+      <c r="G137" s="2">
+        <v>0.50367961999999999</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="1">
+        <v>136</v>
+      </c>
+      <c r="B138" s="1">
+        <v>724.35</v>
+      </c>
+      <c r="C138" s="1">
+        <v>724.07</v>
+      </c>
+      <c r="D138" s="1">
+        <v>2342.73</v>
+      </c>
+      <c r="E138" s="1">
+        <v>72.37</v>
+      </c>
+      <c r="F138" s="1">
+        <v>52.67</v>
+      </c>
+      <c r="G138" s="2">
+        <v>0.61551418000000002</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="1">
+        <v>137</v>
+      </c>
+      <c r="B139" s="1">
+        <v>724.35</v>
+      </c>
+      <c r="C139" s="1">
+        <v>682.51</v>
+      </c>
+      <c r="D139" s="1">
+        <v>2415.3000000000002</v>
+      </c>
+      <c r="E139" s="1">
+        <v>72.37</v>
+      </c>
+      <c r="F139" s="1">
+        <v>57.52</v>
+      </c>
+      <c r="G139" s="2">
+        <v>0.55187162999999995</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="1">
+        <v>138</v>
+      </c>
+      <c r="B140" s="1">
+        <v>732.79</v>
+      </c>
+      <c r="C140" s="1">
+        <v>681.22</v>
+      </c>
+      <c r="D140" s="1">
+        <v>2391.27</v>
+      </c>
+      <c r="E140" s="1">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="F140" s="1">
+        <v>57.69</v>
+      </c>
+      <c r="G140" s="2">
+        <v>0.55418290000000003</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="1">
+        <v>139</v>
+      </c>
+      <c r="B141" s="1">
+        <v>711.4</v>
+      </c>
+      <c r="C141" s="1">
+        <v>640.74</v>
+      </c>
+      <c r="D141" s="1">
+        <v>2548.15</v>
+      </c>
+      <c r="E141" s="1">
+        <v>76.02</v>
+      </c>
+      <c r="F141" s="1">
+        <v>63.97</v>
+      </c>
+      <c r="G141" s="2">
+        <v>0.56788245999999998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="1">
+        <v>140</v>
+      </c>
+      <c r="B142" s="1">
+        <v>727.4</v>
+      </c>
+      <c r="C142" s="1">
+        <v>747.87</v>
+      </c>
+      <c r="D142" s="1">
+        <v>2294.64</v>
+      </c>
+      <c r="E142" s="1">
+        <v>71.63</v>
+      </c>
+      <c r="F142" s="1">
+        <v>50.34</v>
+      </c>
+      <c r="G142" s="2">
+        <v>0.71425545000000001</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="1">
+        <v>141</v>
+      </c>
+      <c r="B143" s="1">
+        <v>699.33</v>
+      </c>
+      <c r="C143" s="1">
+        <v>652.07000000000005</v>
+      </c>
+      <c r="D143" s="1">
+        <v>2583.2600000000002</v>
+      </c>
+      <c r="E143" s="1">
+        <v>80.8</v>
+      </c>
+      <c r="F143" s="1">
+        <v>62</v>
+      </c>
+      <c r="G143" s="2">
+        <v>0.52802422999999998</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="1">
+        <v>142</v>
+      </c>
+      <c r="B144" s="1">
+        <v>699.33</v>
+      </c>
+      <c r="C144" s="1">
+        <v>639.82000000000005</v>
+      </c>
+      <c r="D144" s="1">
+        <v>2610.31</v>
+      </c>
+      <c r="E144" s="1">
+        <v>80.8</v>
+      </c>
+      <c r="F144" s="1">
+        <v>64.14</v>
+      </c>
+      <c r="G144" s="2">
+        <v>0.55072582999999997</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="1">
+        <v>143</v>
+      </c>
+      <c r="B145" s="1">
+        <v>733.52</v>
+      </c>
+      <c r="C145" s="1">
+        <v>702.77</v>
+      </c>
+      <c r="D145" s="1">
+        <v>2350.21</v>
+      </c>
+      <c r="E145" s="1">
+        <v>70.239999999999995</v>
+      </c>
+      <c r="F145" s="1">
+        <v>55.01</v>
+      </c>
+      <c r="G145" s="2">
+        <v>0.58190299000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="1">
+        <v>144</v>
+      </c>
+      <c r="B146" s="1">
+        <v>734.54</v>
+      </c>
+      <c r="C146" s="1">
+        <v>675.61</v>
+      </c>
+      <c r="D146" s="1">
+        <v>2396.6999999999998</v>
+      </c>
+      <c r="E146" s="1">
+        <v>70.02</v>
+      </c>
+      <c r="F146" s="1">
+        <v>58.45</v>
+      </c>
+      <c r="G146" s="2">
+        <v>0.55081815000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="1">
+        <v>145</v>
+      </c>
+      <c r="B147" s="1">
+        <v>707.45</v>
+      </c>
+      <c r="C147" s="1">
+        <v>717.07</v>
+      </c>
+      <c r="D147" s="1">
+        <v>2419.08</v>
+      </c>
+      <c r="E147" s="1">
+        <v>77.37</v>
+      </c>
+      <c r="F147" s="1">
+        <v>53.41</v>
+      </c>
+      <c r="G147" s="2">
+        <v>0.57639468000000005</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="1">
+        <v>146</v>
+      </c>
+      <c r="B148" s="1">
+        <v>725.65</v>
+      </c>
+      <c r="C148" s="1">
+        <v>654.21</v>
+      </c>
+      <c r="D148" s="1">
+        <v>2466.9</v>
+      </c>
+      <c r="E148" s="1">
+        <v>72.05</v>
+      </c>
+      <c r="F148" s="1">
+        <v>61.65</v>
+      </c>
+      <c r="G148" s="2">
+        <v>0.56042789000000004</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="1">
+        <v>147</v>
+      </c>
+      <c r="B149" s="1">
+        <v>708.26</v>
+      </c>
+      <c r="C149" s="1">
+        <v>736.39</v>
+      </c>
+      <c r="D149" s="1">
+        <v>2383.7199999999998</v>
+      </c>
+      <c r="E149" s="1">
+        <v>77.08</v>
+      </c>
+      <c r="F149" s="1">
+        <v>51.43</v>
+      </c>
+      <c r="G149" s="2">
+        <v>0.63429212000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="1">
+        <v>148</v>
+      </c>
+      <c r="B150" s="1">
+        <v>696.51</v>
+      </c>
+      <c r="C150" s="1">
+        <v>676.92</v>
+      </c>
+      <c r="D150" s="1">
+        <v>2552.59</v>
+      </c>
+      <c r="E150" s="1">
+        <v>82.36</v>
+      </c>
+      <c r="F150" s="1">
+        <v>58.27</v>
+      </c>
+      <c r="G150" s="2">
+        <v>0.50194083</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="1">
+        <v>149</v>
+      </c>
+      <c r="B151" s="1">
+        <v>700.2</v>
+      </c>
+      <c r="C151" s="1">
+        <v>642.16999999999996</v>
+      </c>
+      <c r="D151" s="1">
+        <v>2599.64</v>
+      </c>
+      <c r="E151" s="1">
+        <v>80.37</v>
+      </c>
+      <c r="F151" s="1">
+        <v>63.71</v>
+      </c>
+      <c r="G151" s="2">
+        <v>0.54870878999999995</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="1">
+        <v>150</v>
+      </c>
+      <c r="B152" s="1">
+        <v>713.66</v>
+      </c>
+      <c r="C152" s="1">
+        <v>663.02</v>
+      </c>
+      <c r="D152" s="1">
+        <v>2491.42</v>
+      </c>
+      <c r="E152" s="1">
+        <v>75.31</v>
+      </c>
+      <c r="F152" s="1">
+        <v>60.27</v>
+      </c>
+      <c r="G152" s="2">
+        <v>0.53506577</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="1">
+        <v>151</v>
+      </c>
+      <c r="B153" s="1">
+        <v>703.2</v>
+      </c>
+      <c r="C153" s="1">
+        <v>730.53</v>
+      </c>
+      <c r="D153" s="1">
+        <v>2417.6</v>
+      </c>
+      <c r="E153" s="1">
+        <v>79.02</v>
+      </c>
+      <c r="F153" s="1">
+        <v>52.01</v>
+      </c>
+      <c r="G153" s="2">
+        <v>0.60671691000000005</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="1">
+        <v>152</v>
+      </c>
+      <c r="B154" s="1">
+        <v>713.76</v>
+      </c>
+      <c r="C154" s="1">
+        <v>643.16999999999996</v>
+      </c>
+      <c r="D154" s="1">
+        <v>2533.15</v>
+      </c>
+      <c r="E154" s="1">
+        <v>75.28</v>
+      </c>
+      <c r="F154" s="1">
+        <v>63.53</v>
+      </c>
+      <c r="G154" s="2">
+        <v>0.56599666999999998</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="1">
+        <v>153</v>
+      </c>
+      <c r="B155" s="1">
+        <v>732.38</v>
+      </c>
+      <c r="C155" s="1">
+        <v>718.93</v>
+      </c>
+      <c r="D155" s="1">
+        <v>2326.04</v>
+      </c>
+      <c r="E155" s="1">
+        <v>70.489999999999995</v>
+      </c>
+      <c r="F155" s="1">
+        <v>53.21</v>
+      </c>
+      <c r="G155" s="2">
+        <v>0.60469521000000004</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="1">
+        <v>154</v>
+      </c>
+      <c r="B156" s="1">
+        <v>715.56</v>
+      </c>
+      <c r="C156" s="1">
+        <v>652.79999999999995</v>
+      </c>
+      <c r="D156" s="1">
+        <v>2505.1799999999998</v>
+      </c>
+      <c r="E156" s="1">
+        <v>74.739999999999995</v>
+      </c>
+      <c r="F156" s="1">
+        <v>61.88</v>
+      </c>
+      <c r="G156" s="2">
+        <v>0.54900592999999998</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="1">
+        <v>155</v>
+      </c>
+      <c r="B157" s="1">
+        <v>731.26</v>
+      </c>
+      <c r="C157" s="1">
+        <v>695.87</v>
+      </c>
+      <c r="D157" s="1">
+        <v>2369.15</v>
+      </c>
+      <c r="E157" s="1">
+        <v>70.739999999999995</v>
+      </c>
+      <c r="F157" s="1">
+        <v>55.83</v>
+      </c>
+      <c r="G157" s="2">
+        <v>0.56868989000000003</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="1">
+        <v>156</v>
+      </c>
+      <c r="B158" s="1">
+        <v>711.65</v>
+      </c>
+      <c r="C158" s="1">
+        <v>710.94</v>
+      </c>
+      <c r="D158" s="1">
+        <v>2411.23</v>
+      </c>
+      <c r="E158" s="1">
+        <v>75.94</v>
+      </c>
+      <c r="F158" s="1">
+        <v>54.08</v>
+      </c>
+      <c r="G158" s="2">
+        <v>0.57582690000000003</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="1">
+        <v>157</v>
+      </c>
+      <c r="B159" s="1">
+        <v>709.8</v>
+      </c>
+      <c r="C159" s="1">
+        <v>732.43</v>
+      </c>
+      <c r="D159" s="1">
+        <v>2383.36</v>
+      </c>
+      <c r="E159" s="1">
+        <v>76.55</v>
+      </c>
+      <c r="F159" s="1">
+        <v>51.82</v>
+      </c>
+      <c r="G159" s="2">
+        <v>0.62493142999999995</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="1">
+        <v>158</v>
+      </c>
+      <c r="B160" s="1">
+        <v>696.11</v>
+      </c>
+      <c r="C160" s="1">
+        <v>647.33000000000004</v>
+      </c>
+      <c r="D160" s="1">
+        <v>2615.77</v>
+      </c>
+      <c r="E160" s="1">
+        <v>82.61</v>
+      </c>
+      <c r="F160" s="1">
+        <v>62.8</v>
+      </c>
+      <c r="G160" s="2">
+        <v>0.52414958</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="1">
+        <v>159</v>
+      </c>
+      <c r="B161" s="1">
+        <v>697.78</v>
+      </c>
+      <c r="C161" s="1">
+        <v>728.55</v>
+      </c>
+      <c r="D161" s="1">
+        <v>2453.0700000000002</v>
+      </c>
+      <c r="E161" s="1">
+        <v>81.62</v>
+      </c>
+      <c r="F161" s="1">
+        <v>52.21</v>
+      </c>
+      <c r="G161" s="2">
+        <v>0.58675973999999997</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="1">
+        <v>160</v>
+      </c>
+      <c r="B162" s="1">
+        <v>694.22</v>
+      </c>
+      <c r="C162" s="1">
+        <v>716.14</v>
+      </c>
+      <c r="D162" s="1">
+        <v>2501.91</v>
+      </c>
+      <c r="E162" s="1">
+        <v>83.93</v>
+      </c>
+      <c r="F162" s="1">
+        <v>53.51</v>
+      </c>
+      <c r="G162" s="2">
+        <v>0.54141691000000003</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="1">
+        <v>161</v>
+      </c>
+      <c r="B163" s="1">
+        <v>695.31</v>
+      </c>
+      <c r="C163" s="1">
+        <v>638.74</v>
+      </c>
+      <c r="D163" s="1">
+        <v>2641.55</v>
+      </c>
+      <c r="E163" s="1">
+        <v>83.14</v>
+      </c>
+      <c r="F163" s="1">
+        <v>64.34</v>
+      </c>
+      <c r="G163" s="2">
+        <v>0.53681484999999995</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="1">
+        <v>162</v>
+      </c>
+      <c r="B164" s="1">
+        <v>695.6</v>
+      </c>
+      <c r="C164" s="1">
+        <v>674.39</v>
+      </c>
+      <c r="D164" s="1">
+        <v>2564.54</v>
+      </c>
+      <c r="E164" s="1">
+        <v>82.94</v>
+      </c>
+      <c r="F164" s="1">
+        <v>58.62</v>
+      </c>
+      <c r="G164" s="2">
+        <v>0.49750473000000001</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="1">
+        <v>163</v>
+      </c>
+      <c r="B165" s="1">
+        <v>696.27</v>
+      </c>
+      <c r="C165" s="1">
+        <v>685.8</v>
+      </c>
+      <c r="D165" s="1">
+        <v>2537.8200000000002</v>
+      </c>
+      <c r="E165" s="1">
+        <v>82.51</v>
+      </c>
+      <c r="F165" s="1">
+        <v>57.09</v>
+      </c>
+      <c r="G165" s="2">
+        <v>0.50983144999999996</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="1">
+        <v>164</v>
+      </c>
+      <c r="B166" s="1">
+        <v>694.42</v>
+      </c>
+      <c r="C166" s="1">
+        <v>724.55</v>
+      </c>
+      <c r="D166" s="1">
+        <v>2486.08</v>
+      </c>
+      <c r="E166" s="1">
+        <v>83.78</v>
+      </c>
+      <c r="F166" s="1">
+        <v>52.62</v>
+      </c>
+      <c r="G166" s="2">
+        <v>0.55772988999999995</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="1">
+        <v>165</v>
+      </c>
+      <c r="B167" s="1">
+        <v>697.8</v>
+      </c>
+      <c r="C167" s="1">
+        <v>750.05</v>
+      </c>
+      <c r="D167" s="1">
+        <v>2418.66</v>
+      </c>
+      <c r="E167" s="1">
+        <v>81.61</v>
+      </c>
+      <c r="F167" s="1">
+        <v>50.14</v>
+      </c>
+      <c r="G167" s="2">
+        <v>0.68403205</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="1">
+        <v>166</v>
+      </c>
+      <c r="B168" s="1">
+        <v>708.01</v>
+      </c>
+      <c r="C168" s="1">
+        <v>738.35</v>
+      </c>
+      <c r="D168" s="1">
+        <v>2381.7199999999998</v>
+      </c>
+      <c r="E168" s="1">
+        <v>77.17</v>
+      </c>
+      <c r="F168" s="1">
+        <v>51.24</v>
+      </c>
+      <c r="G168" s="2">
+        <v>0.64274224000000002</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="1">
+        <v>167</v>
+      </c>
+      <c r="B169" s="1">
+        <v>702.59</v>
+      </c>
+      <c r="C169" s="1">
+        <v>708.27</v>
+      </c>
+      <c r="D169" s="1">
+        <v>2458.0100000000002</v>
+      </c>
+      <c r="E169" s="1">
+        <v>79.28</v>
+      </c>
+      <c r="F169" s="1">
+        <v>54.38</v>
+      </c>
+      <c r="G169" s="2">
+        <v>0.55900671999999996</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="1">
+        <v>168</v>
+      </c>
+      <c r="B170" s="1">
+        <v>693.75</v>
+      </c>
+      <c r="C170" s="1">
+        <v>670.08</v>
+      </c>
+      <c r="D170" s="1">
+        <v>2589.61</v>
+      </c>
+      <c r="E170" s="1">
+        <v>84.31</v>
+      </c>
+      <c r="F170" s="1">
+        <v>59.23</v>
+      </c>
+      <c r="G170" s="2">
+        <v>0.48851489999999997</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="1">
+        <v>169</v>
+      </c>
+      <c r="B171" s="1">
+        <v>708.89</v>
+      </c>
+      <c r="C171" s="1">
+        <v>663.68</v>
+      </c>
+      <c r="D171" s="1">
+        <v>2509.91</v>
+      </c>
+      <c r="E171" s="1">
+        <v>76.86</v>
+      </c>
+      <c r="F171" s="1">
+        <v>60.17</v>
+      </c>
+      <c r="G171" s="2">
+        <v>0.52842676</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="1">
+        <v>170</v>
+      </c>
+      <c r="B172" s="1">
+        <v>697.48</v>
+      </c>
+      <c r="C172" s="1">
+        <v>733.75</v>
+      </c>
+      <c r="D172" s="1">
+        <v>2446.73</v>
+      </c>
+      <c r="E172" s="1">
+        <v>81.790000000000006</v>
+      </c>
+      <c r="F172" s="1">
+        <v>51.69</v>
+      </c>
+      <c r="G172" s="2">
+        <v>0.60085142000000002</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="1">
+        <v>171</v>
+      </c>
+      <c r="B173" s="1">
+        <v>720.31</v>
+      </c>
+      <c r="C173" s="1">
+        <v>691.16</v>
+      </c>
+      <c r="D173" s="1">
+        <v>2413.15</v>
+      </c>
+      <c r="E173" s="1">
+        <v>73.41</v>
+      </c>
+      <c r="F173" s="1">
+        <v>56.41</v>
+      </c>
+      <c r="G173" s="2">
+        <v>0.55494319999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>